<commit_message>
login & register DONE .
</commit_message>
<xml_diff>
--- a/UserInfo.xlsx
+++ b/UserInfo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FILLL\OneDrive\Documents\NetBeansProjects\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185DE9F3-1F46-4955-83E5-070E5AD26DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7EDEA5F9-1AD9-4CEA-81A5-EF9D2E73E3AA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{CECEB78C-7C36-4224-9F80-07B50D04883B}"/>
+    <workbookView windowHeight="11388" windowWidth="17280" xWindow="492" xr2:uid="{CECEB78C-7C36-4224-9F80-07B50D04883B}" yWindow="852"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Username</t>
   </si>
@@ -166,15 +166,151 @@
   </si>
   <si>
     <t>089-012-3456</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Fiona</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>Foster</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Mathee</t>
+  </si>
+  <si>
+    <t>R.</t>
+  </si>
+  <si>
+    <t>MatheelnwZa007</t>
+  </si>
+  <si>
+    <t>1234love</t>
+  </si>
+  <si>
+    <t>276 love u 4ever</t>
+  </si>
+  <si>
+    <t>098-765-5432</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>J.op</t>
+  </si>
+  <si>
+    <t>ABC098</t>
+  </si>
+  <si>
+    <t>mmmmm</t>
+  </si>
+  <si>
+    <t>29737feoifeio</t>
+  </si>
+  <si>
+    <t>098-234-1524</t>
+  </si>
+  <si>
+    <t>rrr</t>
+  </si>
+  <si>
+    <t>eeee</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>232erer</t>
+  </si>
+  <si>
+    <t>099-999-9999</t>
+  </si>
+  <si>
+    <t>1234ui</t>
+  </si>
+  <si>
+    <t>jjj</t>
+  </si>
+  <si>
+    <t>IOIO</t>
+  </si>
+  <si>
+    <t>youAndMe1</t>
+  </si>
+  <si>
+    <t>0987abc</t>
+  </si>
+  <si>
+    <t>werwrw</t>
+  </si>
+  <si>
+    <t>076-244-5678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0000000000"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -202,24 +338,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -236,10 +367,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -274,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -326,7 +457,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -437,21 +568,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -468,7 +599,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -520,15 +651,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9951F6-E592-46A9-A836-858479AC9731}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9951F6-E592-46A9-A836-858479AC9731}">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -536,181 +667,314 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D12" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>